<commit_message>
Artefakty z Zad Domowe 1
</commit_message>
<xml_diff>
--- a/Wyniki.xlsx
+++ b/Wyniki.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PRz\Documents\Politechnika Rzeszowska Studenci\Informatyka\InformatykaA1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{088D5E80-08A9-48F4-9C1B-9B812FD258E1}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40883EAE-E6DC-4920-9602-869CF2C1E3BA}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -427,10 +427,10 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1</c:v>
@@ -3539,8 +3539,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -3843,18 +3843,20 @@
       <c r="L7" s="1">
         <v>0</v>
       </c>
-      <c r="M7" s="1"/>
+      <c r="M7" s="1">
+        <v>2.5001000000000002</v>
+      </c>
       <c r="N7" s="1">
         <f>SUM(Tabela1[[#This Row],[Zapoznał się z kartą przedmiotu?]:[Zadanie domowe 1]])</f>
-        <v>9</v>
+        <v>11.5001</v>
       </c>
       <c r="O7" s="1">
         <f>Tabela1[[#This Row],[Suma pkt]]/IF(Tabela1[[#This Row],[+]]=1,$D$17,IF(Tabela1[[#This Row],[+]]=2,$D$18,$D$16))</f>
-        <v>0.6</v>
+        <v>0.76667333333333332</v>
       </c>
       <c r="P7" s="1">
         <f>IF(Tabela1[[#This Row],[%]]&lt;0.6, 2, IF(Tabela1[[#This Row],[%]]&lt;0.7, 3, IF(Tabela1[[#This Row],[%]]&lt;0.8, 3.5, IF(Tabela1[[#This Row],[%]]&lt;0.9, 4, IF(Tabela1[[#This Row],[%]]&lt;0.95, 4.5, 5)))))</f>
-        <v>3</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
@@ -4241,7 +4243,7 @@
       </c>
       <c r="C22">
         <f>COUNTIF(Tabela1[Propozycja oceny],B22)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
@@ -4250,7 +4252,7 @@
       </c>
       <c r="C23">
         <f>COUNTIF(Tabela1[Propozycja oceny],B23)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">

</xml_diff>